<commit_message>
posting in a public repository
</commit_message>
<xml_diff>
--- a/excel_files/Empresas.xlsx
+++ b/excel_files/Empresas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>DOMÍNIO SISTEMAS</t>
   </si>
@@ -33,16 +33,34 @@
     <t>Status</t>
   </si>
   <si>
-    <t>FUSCALDO ADMINISTRA</t>
-  </si>
-  <si>
-    <t>AECI</t>
-  </si>
-  <si>
-    <t>FINK IMOBILIARIA</t>
-  </si>
-  <si>
-    <t>FINK HOLDING</t>
+    <t>AMAZONIA XPRESS</t>
+  </si>
+  <si>
+    <t>FALHA</t>
+  </si>
+  <si>
+    <t>LUZ PUBLICIDADE</t>
+  </si>
+  <si>
+    <t>CONCLUIDO</t>
+  </si>
+  <si>
+    <t>C:\Mia\LUZ-PUBLICIDADE\327.pdf</t>
+  </si>
+  <si>
+    <t>TRANSNACIONAL</t>
+  </si>
+  <si>
+    <t>FALTA DE DADOS</t>
+  </si>
+  <si>
+    <t>JOSEFA ADMIN</t>
+  </si>
+  <si>
+    <t>AHURA MAZDA</t>
+  </si>
+  <si>
+    <t>C:\Mia\AHURA-MAZDA\339.pdf</t>
   </si>
 </sst>
 </file>
@@ -79,14 +97,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,8 +142,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1"/>
+        <fgColor rgb="FFFF6961"/>
         <bgColor rgb="FFFF6961"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF90EE90"/>
+        <bgColor rgb="FF90EE90"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFE0"/>
+        <bgColor rgb="FFFFFFE0"/>
       </patternFill>
     </fill>
   </fills>
@@ -253,10 +284,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -274,28 +306,32 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="4" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -602,24 +638,24 @@
   <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.140625" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" style="16" customWidth="1"/>
+    <col min="4" max="4" width="39.28515625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -628,410 +664,428 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="11">
-        <v>413</v>
-      </c>
-      <c r="C3" s="23"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="19"/>
+      <c r="B3" s="12">
+        <v>423</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="12"/>
+      <c r="F3" s="14"/>
       <c r="G3" s="9"/>
-      <c r="H3" s="19"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="12">
+        <v>327</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="12">
+        <v>61</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="14"/>
+    </row>
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="12">
+        <v>380</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="11">
-        <v>346</v>
-      </c>
-      <c r="C4" s="23"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="19"/>
-    </row>
-    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="11">
-        <v>373</v>
-      </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="19"/>
-    </row>
-    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="14"/>
+    </row>
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3">
+        <v>339</v>
+      </c>
+      <c r="C7" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="11">
-        <v>371</v>
-      </c>
-      <c r="C6" s="23"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="19"/>
-    </row>
-    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="11"/>
-      <c r="C7" s="18"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
+      <c r="D7" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="19"/>
+      <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="11"/>
-      <c r="C8" s="18"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="19"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="14"/>
     </row>
     <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
-      <c r="C9" s="18"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="20"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="19"/>
+      <c r="H9" s="14"/>
     </row>
     <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="18"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="20"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="19"/>
+      <c r="H10" s="14"/>
     </row>
     <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="11"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="13"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="19"/>
+      <c r="H11" s="14"/>
     </row>
     <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="11"/>
-      <c r="C12" s="18"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="20"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="19"/>
+      <c r="H12" s="14"/>
     </row>
     <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="11"/>
-      <c r="C13" s="18"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="20"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
       <c r="G13" s="9"/>
-      <c r="H13" s="19"/>
+      <c r="H13" s="14"/>
     </row>
     <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
-      <c r="C14" s="18"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="20"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="19"/>
+      <c r="H14" s="14"/>
     </row>
     <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="11"/>
-      <c r="C15" s="18"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="20"/>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
       <c r="G15" s="9"/>
-      <c r="H15" s="19"/>
+      <c r="H15" s="14"/>
     </row>
     <row r="16" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="11"/>
-      <c r="C16" s="18"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="20"/>
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
-      <c r="H16" s="19"/>
+      <c r="H16" s="14"/>
     </row>
     <row r="17" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="11"/>
-      <c r="C17" s="18"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="20"/>
       <c r="E17" s="9"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="19"/>
+      <c r="H17" s="14"/>
     </row>
     <row r="18" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="11"/>
-      <c r="C18" s="18"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="20"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
     </row>
     <row r="19" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="11"/>
-      <c r="C19" s="18"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="20"/>
     </row>
     <row r="20" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="11"/>
-      <c r="C20" s="18"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="20"/>
     </row>
     <row r="21" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="11"/>
-      <c r="C21" s="18"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="20"/>
     </row>
     <row r="22" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="11"/>
-      <c r="C22" s="18"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="20"/>
     </row>
     <row r="23" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="11"/>
-      <c r="C23" s="18"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="20"/>
     </row>
     <row r="24" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="11"/>
-      <c r="C24" s="18"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="20"/>
     </row>
     <row r="25" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="11"/>
-      <c r="C25" s="18"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="20"/>
     </row>
     <row r="26" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="11"/>
-      <c r="C26" s="18"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="20"/>
     </row>
     <row r="27" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="11"/>
-      <c r="C27" s="18"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="20"/>
     </row>
     <row r="28" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="11"/>
-      <c r="C28" s="18"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="20"/>
     </row>
     <row r="29" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="11"/>
-      <c r="C29" s="18"/>
-      <c r="E29" s="11"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="20"/>
+      <c r="E29" s="12"/>
     </row>
     <row r="30" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="11"/>
-      <c r="C30" s="18"/>
+      <c r="B30" s="12"/>
+      <c r="C30" s="20"/>
     </row>
     <row r="31" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="11"/>
-      <c r="C31" s="18"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="20"/>
     </row>
     <row r="32" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="11"/>
-      <c r="C32" s="18"/>
+      <c r="B32" s="12"/>
+      <c r="C32" s="20"/>
     </row>
     <row r="33" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="11"/>
-      <c r="C33" s="18"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="20"/>
     </row>
     <row r="34" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="11"/>
-      <c r="C34" s="18"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="20"/>
     </row>
     <row r="35" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="11"/>
-      <c r="C35" s="18"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="20"/>
     </row>
     <row r="36" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="11"/>
-      <c r="C36" s="18"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="20"/>
     </row>
     <row r="37" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="11"/>
-      <c r="C37" s="18"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="20"/>
     </row>
     <row r="38" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="11"/>
-      <c r="C38" s="18"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="20"/>
     </row>
     <row r="39" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="11"/>
-      <c r="C39" s="18"/>
+      <c r="B39" s="12"/>
+      <c r="C39" s="20"/>
     </row>
     <row r="40" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="11"/>
-      <c r="C40" s="18"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="20"/>
     </row>
     <row r="41" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="11"/>
-      <c r="C41" s="18"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="20"/>
     </row>
     <row r="42" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="11"/>
-      <c r="C42" s="18"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="20"/>
     </row>
     <row r="43" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="11"/>
-      <c r="C43" s="18"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="20"/>
     </row>
     <row r="44" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="11"/>
-      <c r="C44" s="18"/>
+      <c r="B44" s="12"/>
+      <c r="C44" s="20"/>
     </row>
     <row r="45" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="11"/>
-      <c r="C45" s="18"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="20"/>
     </row>
     <row r="46" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="11"/>
-      <c r="C46" s="18"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="20"/>
     </row>
     <row r="47" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="11"/>
-      <c r="C47" s="18"/>
+      <c r="B47" s="12"/>
+      <c r="C47" s="20"/>
     </row>
     <row r="48" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="11"/>
-      <c r="C48" s="18"/>
+      <c r="B48" s="12"/>
+      <c r="C48" s="20"/>
     </row>
     <row r="49" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="11"/>
-      <c r="C49" s="18"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="20"/>
     </row>
     <row r="50" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="11"/>
-      <c r="C50" s="18"/>
+      <c r="B50" s="12"/>
+      <c r="C50" s="20"/>
     </row>
     <row r="51" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="11"/>
-      <c r="C51" s="18"/>
+      <c r="B51" s="12"/>
+      <c r="C51" s="20"/>
     </row>
     <row r="52" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="11"/>
-      <c r="C52" s="18"/>
+      <c r="B52" s="12"/>
+      <c r="C52" s="20"/>
     </row>
     <row r="53" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="11"/>
-      <c r="C53" s="18"/>
+      <c r="B53" s="12"/>
+      <c r="C53" s="20"/>
     </row>
     <row r="54" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="11"/>
-      <c r="C54" s="18"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="20"/>
     </row>
     <row r="55" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="11"/>
-      <c r="C55" s="18"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="20"/>
     </row>
     <row r="56" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="11"/>
-      <c r="C56" s="18"/>
+      <c r="B56" s="12"/>
+      <c r="C56" s="20"/>
     </row>
     <row r="57" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="11"/>
-      <c r="C57" s="18"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="20"/>
     </row>
     <row r="58" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="11"/>
-      <c r="C58" s="18"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="20"/>
     </row>
     <row r="59" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="11"/>
-      <c r="C59" s="18"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="20"/>
     </row>
     <row r="60" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="11"/>
-      <c r="C60" s="18"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="20"/>
     </row>
     <row r="61" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="11"/>
-      <c r="C61" s="18"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="20"/>
     </row>
     <row r="62" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="11"/>
-      <c r="C62" s="18"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="20"/>
     </row>
     <row r="63" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="11"/>
-      <c r="C63" s="18"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="20"/>
     </row>
     <row r="64" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="11"/>
-      <c r="C64" s="18"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="20"/>
     </row>
     <row r="65" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="11"/>
-      <c r="C65" s="18"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="20"/>
     </row>
     <row r="66" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="11"/>
-      <c r="C66" s="18"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="20"/>
     </row>
     <row r="67" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="11"/>
-      <c r="C67" s="18"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="20"/>
     </row>
     <row r="68" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="11"/>
-      <c r="C68" s="18"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="20"/>
     </row>
     <row r="69" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="11"/>
-      <c r="C69" s="18"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="20"/>
     </row>
     <row r="70" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="11"/>
-      <c r="C70" s="18"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="20"/>
     </row>
     <row r="71" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="11"/>
-      <c r="C71" s="18"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="20"/>
       <c r="D71" s="6"/>
     </row>
     <row r="72" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="11"/>
-      <c r="C72" s="18"/>
+      <c r="B72" s="12"/>
+      <c r="C72" s="20"/>
     </row>
     <row r="73" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="11"/>
-      <c r="C73" s="18"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="20"/>
     </row>
     <row r="74" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="11"/>
-      <c r="C74" s="18"/>
+      <c r="B74" s="12"/>
+      <c r="C74" s="20"/>
     </row>
     <row r="75" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="11"/>
-      <c r="C75" s="18"/>
+      <c r="B75" s="12"/>
+      <c r="C75" s="20"/>
     </row>
     <row r="76" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="11"/>
-      <c r="C76" s="18"/>
-      <c r="D76" s="15"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="20"/>
+      <c r="D76" s="18"/>
     </row>
     <row r="77" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="11"/>
-      <c r="C77" s="18"/>
+      <c r="B77" s="12"/>
+      <c r="C77" s="20"/>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C78" s="18"/>
+      <c r="C78" s="20"/>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C79" s="18"/>
+      <c r="C79" s="20"/>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C80" s="18"/>
+      <c r="C80" s="20"/>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C81" s="4"/>
@@ -1100,6 +1154,10 @@
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D7" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>

</xml_diff>